<commit_message>
[doc] added doc and incorrect urls to tests
</commit_message>
<xml_diff>
--- a/docs/simple_url_syntactic_analyzer_table.xlsx
+++ b/docs/simple_url_syntactic_analyzer_table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michal Zajic\workspaces\simple_url_syntactic_analyzer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagyt\Documents\Simple_url_syntactic_analyzer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B44C58B-7E72-457D-987A-68A06454AF88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5021121-7280-4830-951F-265A26659B24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A897444A-ACD6-4F42-A0E0-213A259E14B8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="35">
   <si>
     <t>[A-Za-z]</t>
   </si>
@@ -133,13 +133,16 @@
   </si>
   <si>
     <t>U</t>
+  </si>
+  <si>
+    <t>error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +156,23 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -177,13 +197,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hypertextové prepojenie" xfId="1" builtinId="8"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -199,7 +221,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -498,55 +520,76 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="N22" sqref="A1:N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -560,14 +603,50 @@
       <c r="L2">
         <v>4</v>
       </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
       <c r="M3">
         <v>6</v>
       </c>
@@ -576,8 +655,41 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
       </c>
       <c r="M4">
         <v>8</v>
@@ -587,7 +699,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B5">
@@ -596,10 +708,58 @@
       <c r="C5">
         <v>10</v>
       </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
       </c>
       <c r="G6">
         <v>11</v>
@@ -607,9 +767,27 @@
       <c r="H6">
         <v>12</v>
       </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B7">
@@ -618,17 +796,77 @@
       <c r="C7">
         <v>13</v>
       </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
       </c>
       <c r="E8">
         <v>15</v>
       </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
       <c r="G8">
         <v>14</v>
       </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" t="s">
+        <v>34</v>
+      </c>
       <c r="M8">
         <v>15</v>
       </c>
@@ -637,7 +875,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B9">
@@ -646,10 +884,52 @@
       <c r="C9">
         <v>16</v>
       </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
       </c>
       <c r="E10">
         <v>18</v>
@@ -660,6 +940,21 @@
       <c r="G10">
         <v>18</v>
       </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" t="s">
+        <v>34</v>
+      </c>
       <c r="M10">
         <v>18</v>
       </c>
@@ -668,7 +963,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B11">
@@ -677,9 +972,33 @@
       <c r="C11">
         <v>19</v>
       </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
       <c r="E11">
         <v>19</v>
       </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" t="s">
+        <v>34</v>
+      </c>
       <c r="M11">
         <v>19</v>
       </c>
@@ -688,12 +1007,42 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
       </c>
       <c r="E12">
         <v>20</v>
       </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" t="s">
+        <v>34</v>
+      </c>
       <c r="M12">
         <v>21</v>
       </c>
@@ -702,7 +1051,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B13">
@@ -711,20 +1060,86 @@
       <c r="C13">
         <v>22</v>
       </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
       </c>
       <c r="D14">
         <v>23</v>
       </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" t="s">
+        <v>34</v>
+      </c>
       <c r="N14">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15">
@@ -733,9 +1148,33 @@
       <c r="C15">
         <v>25</v>
       </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
       <c r="E15">
         <v>26</v>
       </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" t="s">
+        <v>34</v>
+      </c>
       <c r="M15">
         <v>26</v>
       </c>
@@ -744,7 +1183,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16">
@@ -753,9 +1192,42 @@
       <c r="C16">
         <v>27</v>
       </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17">
@@ -779,6 +1251,18 @@
       <c r="H17">
         <v>29</v>
       </c>
+      <c r="I17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" t="s">
+        <v>34</v>
+      </c>
       <c r="M17">
         <v>29</v>
       </c>
@@ -787,7 +1271,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B18">
@@ -796,25 +1280,121 @@
       <c r="C18">
         <v>31</v>
       </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
       </c>
       <c r="C19">
         <v>32</v>
       </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" t="s">
+        <v>34</v>
+      </c>
+      <c r="J19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
       </c>
       <c r="C20">
         <v>33</v>
       </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
       <c r="E20">
         <v>34</v>
       </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" t="s">
+        <v>34</v>
+      </c>
       <c r="M20">
         <v>34</v>
       </c>
@@ -823,27 +1403,95 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
       </c>
       <c r="C21">
         <v>35</v>
       </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" t="s">
+        <v>34</v>
+      </c>
+      <c r="N21" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B22">
         <v>36</v>
       </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" t="s">
+        <v>34</v>
+      </c>
+      <c r="N22" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I1" r:id="rId1" xr:uid="{C707D5ED-423A-4D6E-9DEF-CA727B321C4E}"/>
-    <hyperlink ref="J1" r:id="rId2" xr:uid="{4BD779C2-A5BF-4293-A1F7-7CA71204C96D}"/>
-    <hyperlink ref="K1" r:id="rId3" xr:uid="{030741A7-3616-4F03-948E-76A09FF20E28}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>